<commit_message>
update code fix phi coc tu dong tinh
</commit_message>
<xml_diff>
--- a/QuanLyThuVienHUFI/Form_QuanLyThuVien/bin/Debug/phieumuonrs.xlsx
+++ b/QuanLyThuVienHUFI/Form_QuanLyThuVien/bin/Debug/phieumuonrs.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>TRƯỜNG ĐẠI HỌC CÔNG NGHIỆP THỰC PHẨM TP.HCM</t>
   </si>
@@ -44,19 +44,19 @@
     <t>Họ và tên:</t>
   </si>
   <si>
-    <t>Nguyễn Phương Anh Nhật</t>
+    <t>ádasdasd</t>
   </si>
   <si>
     <t>Mã số thẻ:</t>
   </si>
   <si>
-    <t>2033207524</t>
+    <t>21381723123</t>
   </si>
   <si>
     <t xml:space="preserve">Phí cọc: </t>
   </si>
   <si>
-    <t>260000 đồng</t>
+    <t>1112000 đồng</t>
   </si>
   <si>
     <t>Tên tài liệu</t>
@@ -68,16 +68,22 @@
     <t>KH xếp giá</t>
   </si>
   <si>
-    <t>The Langmaster - Luyện Kỹ Năng Nghe-Nói-Đọc-Viết Tiếng Anh (Tái Bản 2018)</t>
-  </si>
-  <si>
-    <t>Trần Mạnh Tường</t>
-  </si>
-  <si>
-    <t>B-400</t>
-  </si>
-  <si>
-    <t>TP. Hồ Chí Minh, Ngày 17 tháng 1 năm 2021.</t>
+    <t>Enzyme Chống Lão Hóa (Tái Bản 2020)</t>
+  </si>
+  <si>
+    <t>Hiromi Shinya</t>
+  </si>
+  <si>
+    <t>B-300</t>
+  </si>
+  <si>
+    <t>Street Of Eternal Happiness: Big City Dreams Along A Shanghai Road</t>
+  </si>
+  <si>
+    <t>Rob Schmitz</t>
+  </si>
+  <si>
+    <t>TP. Hồ Chí Minh, Ngày 18 tháng 1 năm 2021.</t>
   </si>
   <si>
     <t>Người mượn</t>
@@ -604,9 +610,15 @@
     </row>
     <row r="13" ht="24.6" customHeight="1">
       <c r="A13" s="13"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="B13" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" ht="25.8" customHeight="1">
       <c r="A14" s="13"/>
@@ -617,13 +629,13 @@
     <row r="15" ht="24" customHeight="1"/>
     <row r="16" ht="15.6">
       <c r="C16" s="15" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D16" s="15"/>
     </row>
     <row r="17" ht="15.6">
       <c r="C17" s="19" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="8"/>

</xml_diff>

<commit_message>
update msg phi coc
</commit_message>
<xml_diff>
--- a/QuanLyThuVienHUFI/Form_QuanLyThuVien/bin/Debug/phieumuonrs.xlsx
+++ b/QuanLyThuVienHUFI/Form_QuanLyThuVien/bin/Debug/phieumuonrs.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>TRƯỜNG ĐẠI HỌC CÔNG NGHIỆP THỰC PHẨM TP.HCM</t>
   </si>
@@ -56,7 +56,7 @@
     <t xml:space="preserve">Phí cọc: </t>
   </si>
   <si>
-    <t>1112000 đồng</t>
+    <t>240000 đồng</t>
   </si>
   <si>
     <t>Tên tài liệu</t>
@@ -75,12 +75,6 @@
   </si>
   <si>
     <t>B-300</t>
-  </si>
-  <si>
-    <t>Street Of Eternal Happiness: Big City Dreams Along A Shanghai Road</t>
-  </si>
-  <si>
-    <t>Rob Schmitz</t>
   </si>
   <si>
     <t>TP. Hồ Chí Minh, Ngày 18 tháng 1 năm 2021.</t>
@@ -610,15 +604,9 @@
     </row>
     <row r="13" ht="24.6" customHeight="1">
       <c r="A13" s="13"/>
-      <c r="B13" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" ht="25.8" customHeight="1">
       <c r="A14" s="13"/>
@@ -629,13 +617,13 @@
     <row r="15" ht="24" customHeight="1"/>
     <row r="16" ht="15.6">
       <c r="C16" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D16" s="15"/>
     </row>
     <row r="17" ht="15.6">
       <c r="C17" s="19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="8"/>

</xml_diff>